<commit_message>
CRUD, Sync Landing Page
</commit_message>
<xml_diff>
--- a/PREPARECTI.xlsx
+++ b/PREPARECTI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Laravel\cti_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401DE431-5A95-484A-9E79-F766E228CE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3826FE1-6447-4B3B-8631-15D18C0C6822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2352A5E9-D46C-43FB-B189-5BFE52A39EDE}"/>
   </bookViews>
@@ -219,7 +219,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,11 +246,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -472,44 +467,44 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,27 +536,27 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,11 +633,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -656,14 +650,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
@@ -672,7 +671,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BB4C989-C4D9-461B-9B30-2BD96C75805A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -712,20 +711,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
@@ -734,7 +738,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77269608-9787-43C1-8850-93E8C4922464}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -774,20 +778,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
@@ -796,7 +805,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD8E669-276F-4E67-93BA-87DE0BCDB411}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -836,20 +845,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -858,7 +872,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AEF079-C20C-4FE2-BFFF-7C1AA820FCD3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -898,20 +912,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -920,7 +939,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{419C9E38-1633-4032-B57D-FA5DF9CF1BB1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -960,20 +979,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -982,7 +1006,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D030EA10-6E58-4BD8-8080-157F5621F202}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -999,11 +1023,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1011,20 +1034,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -1033,7 +1061,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C605DEE9-C5F9-46F8-B900-F4B062C15156}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1050,11 +1078,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1062,20 +1089,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -1084,7 +1116,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90EF4C1-11B6-4E6B-AEDA-F55E6C8EB7EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1101,11 +1133,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1113,20 +1144,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1135,7 +1171,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A22B14C7-4555-47C1-8CB3-4C415D3FFE29}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1152,11 +1188,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1164,20 +1199,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1186,7 +1226,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCD4E035-645A-4F42-88BC-53A0773670FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1203,11 +1243,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1215,20 +1254,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -1237,7 +1281,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3E73208-B586-4F49-A30C-AA8AEB7EA20C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1254,11 +1298,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1266,20 +1309,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
@@ -1288,7 +1336,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F1FC4AE-2D74-444C-9C81-F84257E1D30B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1305,11 +1353,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1317,20 +1364,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
@@ -1339,7 +1391,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2649E4-12F0-4C63-891B-A56C18A8C5CC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1356,11 +1408,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1368,20 +1419,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
@@ -1390,7 +1446,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C63565-76F7-4FAB-A6B2-A8D91581E0D2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1407,11 +1463,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1419,20 +1474,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
@@ -1441,7 +1501,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509AD066-8AF6-4D94-9EAF-1EF8F370D1BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1458,11 +1518,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1470,20 +1529,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
           <xdr:colOff>198120</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="205740" cy="236220"/>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>403860</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
@@ -1492,7 +1556,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46724C28-7CA6-4C3E-B014-7ECEFA76C31B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1509,11 +1573,10 @@
             <a:solidFill>
               <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="008000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="17"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -1521,7 +1584,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2155,7 +2218,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O6"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,50 +2234,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="F1" s="25" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="K1" s="25" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="K1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="35"/>
+      <c r="F2" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="K2" s="27" t="s">
+      <c r="I2" s="37"/>
+      <c r="K2" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29" t="s">
+      <c r="L2" s="34"/>
+      <c r="M2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="30"/>
+      <c r="N2" s="37"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -2255,37 +2318,37 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
+      <c r="A4" s="31">
         <v>1</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="31">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="28" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="28">
         <v>3</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="28">
         <v>2</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="28" t="s">
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="28">
         <v>5</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="28">
         <v>4</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="28" t="s">
         <v>55</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -2293,29 +2356,29 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="32"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
@@ -2331,21 +2394,21 @@
       <c r="I6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
       <c r="N6" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
+      <c r="A7" s="25">
         <v>2</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="25">
         <v>1</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="28" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2357,17 +2420,17 @@
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="32"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="3" t="s">
         <v>48</v>
       </c>
@@ -2378,11 +2441,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="A1:D1"/>
@@ -2393,12 +2457,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>